<commit_message>
new file:   LAB_20200225_0_TrafficLight/LAB_20200225_0/EAGLE/Module 20200225_0_Traffic Light.sch         new file:   LAB_20200225_0_TrafficLight/LAB_20200225_0/LAB_20200225_0.xlsx         new file:   LAB_20200622_0_Dispenser/LAB_20200622_0_Dispenser.xlsx         modified:   Lesson_20200612_0_Breadboard/Lesson_20200612_0_Breadboard.xlsx         new file:   Lesson_20200701_0_ArduinoIDE101/Lesson_20200701_0_ArduinoIDE101.pptx         new file:   Lesson_20200701_0_ArduinoIDE101/Lesson_20200701_0_ArduinoIDE101.xlsx         new file:   Lesson_20200703_0_TrafficLight/Lesson_20200703_0_TrafficLight.pptx         new file:   Lesson_20200703_0_TrafficLight/Lesson_20200703_0_TrafficLight.xlsx         modified:   Project_RPSRobot_20200330_0/Project_RPSRobot_20200330_0.xlsx
</commit_message>
<xml_diff>
--- a/Lesson_20200612_0_Breadboard/Lesson_20200612_0_Breadboard.xlsx
+++ b/Lesson_20200612_0_Breadboard/Lesson_20200612_0_Breadboard.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a59c1bdb761853cd/NAER/EELAB/EELAB/Lesson_20200612_0_Breadboard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="138" documentId="11_F25DC773A252ABDACC1048E0995B61245BDE58ED" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0EF02D70-7E79-4F65-B058-0EBFD99074D1}"/>
+  <xr:revisionPtr revIDLastSave="152" documentId="11_F25DC773A252ABDACC1048E0995B61245BDE58ED" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{394AB3DD-9F38-476B-9002-EE92F5558AEA}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="History" sheetId="5" r:id="rId1"/>
@@ -1671,7 +1671,7 @@
       <xdr:row>30</xdr:row>
       <xdr:rowOff>160020</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="6650218" cy="1131400"/>
+    <xdr:ext cx="6934975" cy="1707390"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="24" name="文字方塊 23">
@@ -1686,7 +1686,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="693420" y="5875020"/>
-          <a:ext cx="6650218" cy="1131400"/>
+          <a:ext cx="6934975" cy="1707390"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1798,6 +1798,67 @@
           <a:r>
             <a:rPr lang="zh-TW" altLang="en-US" sz="1200"/>
             <a:t>同學間可以互相討論教學</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="zh-TW" sz="1200"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" altLang="zh-TW" sz="1200"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-TW" sz="1200"/>
+            <a:t>3.</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-TW" altLang="en-US" sz="1200"/>
+            <a:t>競賽題時可以允許</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-TW" sz="1200"/>
+            <a:t>(</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-TW" altLang="en-US" sz="1200"/>
+            <a:t>或規定</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-TW" sz="1200"/>
+            <a:t>)</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-TW" altLang="en-US" sz="1200"/>
+            <a:t>學生於比賽時更換棒次順序</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-TW" sz="1200"/>
+            <a:t>,</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-TW" altLang="en-US" sz="1200"/>
+            <a:t>但練習題時則不建議</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-TW" sz="1200"/>
+            <a:t>,</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-TW" altLang="en-US" sz="1200"/>
+            <a:t>保留完整的學生繪圖及</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="zh-TW" sz="1200"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="zh-TW" altLang="en-US" sz="1200"/>
+            <a:t>接線</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-TW" sz="1200"/>
+            <a:t>,</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-TW" altLang="en-US" sz="1200"/>
+            <a:t>方便小組討論</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -2345,8 +2406,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEB7F64C-6FEE-4994-B373-83D8D21E04D5}">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -2558,8 +2619,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{522DE6CA-1630-4C9F-8AF5-084E560FF0EA}">
   <dimension ref="B6:U19"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:U19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>

</xml_diff>